<commit_message>
anon student id homogenise to all str - previously some were str and some int - this caused duplicate student id to appear - fixed these, changed output.xlsx - obtained performance plot for the non-duplicated df
</commit_message>
<xml_diff>
--- a/Data/output.xlsx
+++ b/Data/output.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F178"/>
+  <dimension ref="A1:F172"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2016,13 +2016,13 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="E69" t="n">
-        <v>33</v>
+        <v>80</v>
       </c>
       <c r="F69" t="n">
-        <v>90.90909090909091</v>
+        <v>73.75</v>
       </c>
     </row>
     <row r="70">
@@ -2040,13 +2040,13 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E70" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F70" t="n">
-        <v>100</v>
+        <v>64.70588235294117</v>
       </c>
     </row>
     <row r="71">
@@ -2064,13 +2064,13 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="E71" t="n">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="F71" t="n">
-        <v>68.75</v>
+        <v>72.72727272727273</v>
       </c>
     </row>
     <row r="72">
@@ -2136,13 +2136,13 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="E74" t="n">
-        <v>54</v>
+        <v>109</v>
       </c>
       <c r="F74" t="n">
-        <v>44.44444444444444</v>
+        <v>59.63302752293578</v>
       </c>
     </row>
     <row r="75">
@@ -2232,13 +2232,13 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E78" t="n">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="F78" t="n">
-        <v>55.55555555555556</v>
+        <v>56.81818181818182</v>
       </c>
     </row>
     <row r="79">
@@ -2256,21 +2256,23 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="E79" t="n">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="F79" t="n">
-        <v>100</v>
+        <v>81.66666666666667</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="B80" t="n">
-        <v>6111001842</v>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>6111001842</t>
+        </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -2291,8 +2293,10 @@
       <c r="A81" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="B81" t="n">
-        <v>6111001842</v>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>6111001842</t>
+        </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -2313,8 +2317,10 @@
       <c r="A82" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="B82" t="n">
-        <v>6111001842</v>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>6111001842</t>
+        </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -2335,118 +2341,130 @@
       <c r="A83" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="B83" t="n">
-        <v>6111001842</v>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>6111001842</t>
+        </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL4.decr.17</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF2-BL4.incr.5</t>
         </is>
       </c>
       <c r="D83" t="n">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="E83" t="n">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="F83" t="n">
-        <v>14.28571428571429</v>
+        <v>58.97435897435897</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="B84" t="n">
-        <v>6111001842</v>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>6111001842</t>
+        </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF2-BL4.incr.5</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL3.incr.2</t>
         </is>
       </c>
       <c r="D84" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="E84" t="n">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="F84" t="n">
-        <v>58.97435897435897</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="B85" t="n">
-        <v>6111001842</v>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>6111001842</t>
+        </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL2.decr.19</t>
+          <t>bpop.num_0..9.by.1.asc.q2q.AV.rise.12__it_2</t>
         </is>
       </c>
       <c r="D85" t="n">
         <v>15</v>
       </c>
       <c r="E85" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F85" t="n">
-        <v>57.69230769230769</v>
+        <v>68.18181818181819</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
         <v>84</v>
       </c>
-      <c r="B86" t="n">
-        <v>6111001842</v>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>6111001995</t>
+        </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL3.decr.18</t>
+          <t>bpop.gl_num.0..9.GL_SD_OFFW1_L.bub3.16</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E86" t="n">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="F86" t="n">
-        <v>61.70212765957447</v>
+        <v>64.70588235294117</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="B87" t="n">
-        <v>6111001842</v>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>6111001995</t>
+        </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL2.incr.3</t>
+          <t>bpop.num_0..9.by.1.asc.q2q.AV.rise.12__it_2</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="E87" t="n">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="F87" t="n">
-        <v>78</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="B88" t="n">
-        <v>6111001842</v>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>6111002050</t>
+        </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -2454,1279 +2472,1395 @@
         </is>
       </c>
       <c r="D88" t="n">
-        <v>41</v>
+        <v>183</v>
       </c>
       <c r="E88" t="n">
-        <v>55</v>
+        <v>227</v>
       </c>
       <c r="F88" t="n">
-        <v>74.54545454545455</v>
+        <v>80.61674008810573</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="B89" t="n">
-        <v>6111001842</v>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>6111002050</t>
+        </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL3.incr.2</t>
+          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL2.decr.19</t>
         </is>
       </c>
       <c r="D89" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="E89" t="n">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="F89" t="n">
-        <v>12.5</v>
+        <v>45.90163934426229</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="B90" t="n">
-        <v>6111001842</v>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>6111002050</t>
+        </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL1.incr.4</t>
+          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL3.decr.18</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="E90" t="n">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="F90" t="n">
-        <v>83.33333333333333</v>
+        <v>47.43589743589744</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="B91" t="n">
-        <v>6111001842</v>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>6111002050</t>
+        </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.asc.q2q.AV.rise.12__it_2</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL1.incr.4</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E91" t="n">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F91" t="n">
-        <v>68.18181818181819</v>
+        <v>73.52941176470588</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="B92" t="n">
-        <v>6111001995</v>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>6111002050</t>
+        </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>bpop.gl_num.0..9.GL_SD_OFFW1_L.bub3.16</t>
+          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL4.decr.17</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>11</v>
+        <v>110</v>
       </c>
       <c r="E92" t="n">
-        <v>17</v>
+        <v>137</v>
       </c>
       <c r="F92" t="n">
-        <v>64.70588235294117</v>
+        <v>80.29197080291971</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
         <v>91</v>
       </c>
-      <c r="B93" t="n">
-        <v>6111001995</v>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>6111002050</t>
+        </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.asc.q2q.AV.rise.12__it_2</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF2-BL4.incr.5</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E93" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F93" t="n">
-        <v>37.5</v>
+        <v>80</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="B94" t="n">
-        <v>6111002050</v>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>6111002050</t>
+        </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL1.decr.20</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF2-BL3.incr.6</t>
         </is>
       </c>
       <c r="D94" t="n">
-        <v>183</v>
+        <v>103</v>
       </c>
       <c r="E94" t="n">
-        <v>227</v>
+        <v>166</v>
       </c>
       <c r="F94" t="n">
-        <v>80.61674008810573</v>
+        <v>62.04819277108434</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
         <v>93</v>
       </c>
-      <c r="B95" t="n">
-        <v>6111002050</v>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>6111002050</t>
+        </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL2.decr.19</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL4.incr.1</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="E95" t="n">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="F95" t="n">
-        <v>45.90163934426229</v>
+        <v>55.55555555555556</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
         <v>94</v>
       </c>
-      <c r="B96" t="n">
-        <v>6111002050</v>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>6111002050</t>
+        </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL3.decr.18</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL3.incr.2</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E96" t="n">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="F96" t="n">
-        <v>47.43589743589744</v>
+        <v>61.19402985074627</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
         <v>95</v>
       </c>
-      <c r="B97" t="n">
-        <v>6111002050</v>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>6111002050</t>
+        </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL1.incr.4</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF5-BL3.incr.10</t>
         </is>
       </c>
       <c r="D97" t="n">
-        <v>25</v>
+        <v>155</v>
       </c>
       <c r="E97" t="n">
-        <v>34</v>
+        <v>198</v>
       </c>
       <c r="F97" t="n">
-        <v>73.52941176470588</v>
+        <v>78.28282828282828</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
         <v>96</v>
       </c>
-      <c r="B98" t="n">
-        <v>6111002050</v>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>6111002050</t>
+        </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL4.decr.17</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF5-BL4.incr.9</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>110</v>
+        <v>33</v>
       </c>
       <c r="E98" t="n">
-        <v>137</v>
+        <v>36</v>
       </c>
       <c r="F98" t="n">
-        <v>80.29197080291971</v>
+        <v>91.66666666666667</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
         <v>97</v>
       </c>
-      <c r="B99" t="n">
-        <v>6111002050</v>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>6111002050</t>
+        </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF2-BL4.incr.5</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF5-BL2.incr.11</t>
         </is>
       </c>
       <c r="D99" t="n">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="E99" t="n">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="F99" t="n">
-        <v>80</v>
+        <v>62.12121212121212</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
         <v>98</v>
       </c>
-      <c r="B100" t="n">
-        <v>6111002050</v>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>6111002050</t>
+        </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF2-BL3.incr.6</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF2-BL1.incr.8</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>103</v>
+        <v>7</v>
       </c>
       <c r="E100" t="n">
-        <v>166</v>
+        <v>18</v>
       </c>
       <c r="F100" t="n">
-        <v>62.04819277108434</v>
+        <v>38.88888888888889</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="B101" t="n">
-        <v>6111002050</v>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>6111002050</t>
+        </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL4.incr.1</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF5-BL1.incr.12</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E101" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F101" t="n">
-        <v>55.55555555555556</v>
+        <v>21.73913043478261</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="B102" t="n">
-        <v>6111002050</v>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>6111002050</t>
+        </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL3.incr.2</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF2-BL2.incr.7</t>
         </is>
       </c>
       <c r="D102" t="n">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="E102" t="n">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="F102" t="n">
-        <v>61.19402985074627</v>
+        <v>58.25242718446602</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="B103" t="n">
-        <v>6111002050</v>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>6111002050</t>
+        </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF5-BL3.incr.10</t>
+          <t>bpop.num_0..9.by.1.asc.q2q.AV.rise.12__it_2</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>155</v>
+        <v>30</v>
       </c>
       <c r="E103" t="n">
-        <v>198</v>
+        <v>37</v>
       </c>
       <c r="F103" t="n">
-        <v>78.28282828282828</v>
+        <v>81.08108108108108</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="B104" t="n">
-        <v>6111002050</v>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>6111002050</t>
+        </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF5-BL4.incr.9</t>
+          <t>bpop.num_0..9.by.1.rand.x2s.Ax.rise.42__it_2</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="E104" t="n">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="F104" t="n">
-        <v>91.66666666666667</v>
+        <v>100</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
         <v>103</v>
       </c>
-      <c r="B105" t="n">
-        <v>6111002050</v>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>6111002050</t>
+        </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF5-BL2.incr.11</t>
+          <t>bpop.gl_num.0..9.GL_SD_OFFW1_L.bub3.16</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="E105" t="n">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="F105" t="n">
-        <v>62.12121212121212</v>
+        <v>82.35294117647059</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
         <v>104</v>
       </c>
-      <c r="B106" t="n">
-        <v>6111002050</v>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>6113001685</t>
+        </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF2-BL1.incr.8</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL2.incr.3</t>
         </is>
       </c>
       <c r="D106" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E106" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F106" t="n">
-        <v>38.88888888888889</v>
+        <v>90.90909090909091</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="B107" t="n">
-        <v>6111002050</v>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>6113001685</t>
+        </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF5-BL1.incr.12</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL1.incr.4</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="E107" t="n">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="F107" t="n">
-        <v>21.73913043478261</v>
+        <v>80.70175438596492</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
         <v>106</v>
       </c>
-      <c r="B108" t="n">
-        <v>6111002050</v>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>6113001685</t>
+        </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF2-BL2.incr.7</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL3.incr.2</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>60</v>
+        <v>3</v>
       </c>
       <c r="E108" t="n">
-        <v>103</v>
+        <v>4</v>
       </c>
       <c r="F108" t="n">
-        <v>58.25242718446602</v>
+        <v>75</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
         <v>107</v>
       </c>
-      <c r="B109" t="n">
-        <v>6111002050</v>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>6113001685</t>
+        </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.asc.q2q.AV.rise.12__it_2</t>
+          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL3.decr.18</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E109" t="n">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="F109" t="n">
-        <v>81.08108108108108</v>
+        <v>66.66666666666667</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
         <v>108</v>
       </c>
-      <c r="B110" t="n">
-        <v>6111002050</v>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>6113001685</t>
+        </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.rand.x2s.Ax.rise.42__it_2</t>
+          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL4.decr.17</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E110" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F110" t="n">
-        <v>100</v>
+        <v>55.55555555555556</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
         <v>109</v>
       </c>
-      <c r="B111" t="n">
-        <v>6111002050</v>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>6113001685</t>
+        </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>bpop.gl_num.0..9.GL_SD_OFFW1_L.bub3.16</t>
+          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL2.decr.19</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E111" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F111" t="n">
-        <v>82.35294117647059</v>
+        <v>83.33333333333333</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="B112" t="n">
-        <v>6113001685</v>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>6113001685</t>
+        </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL2.incr.3</t>
+          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL1.decr.20</t>
         </is>
       </c>
       <c r="D112" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E112" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F112" t="n">
-        <v>90.90909090909091</v>
+        <v>77.77777777777777</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
         <v>111</v>
       </c>
-      <c r="B113" t="n">
-        <v>6113001685</v>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>6113001685</t>
+        </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL1.incr.4</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF5-BL2.incr.11</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="E113" t="n">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="F113" t="n">
-        <v>80.70175438596492</v>
+        <v>66.66666666666667</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
         <v>112</v>
       </c>
-      <c r="B114" t="n">
-        <v>6113001685</v>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>6113001685</t>
+        </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL3.incr.2</t>
+          <t>bpop.mn_4..9.MN-SD-UP-OFF5-BL4.decr.25</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="E114" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="F114" t="n">
-        <v>75</v>
+        <v>95.23809523809524</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
         <v>113</v>
       </c>
-      <c r="B115" t="n">
-        <v>6113001685</v>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>6113001685</t>
+        </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL3.decr.18</t>
+          <t>bpop.mn_4..9.MN-SD-UP-OFF5-BL3.decr.26</t>
         </is>
       </c>
       <c r="D115" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E115" t="n">
         <v>15</v>
       </c>
       <c r="F115" t="n">
-        <v>66.66666666666667</v>
+        <v>80</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
         <v>114</v>
       </c>
-      <c r="B116" t="n">
-        <v>6113001685</v>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>6116001059</t>
+        </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL4.decr.17</t>
+          <t>bpop.mn_10..99.MN-DD-UP-OFF2-BL1.incr.40</t>
         </is>
       </c>
       <c r="D116" t="n">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="E116" t="n">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="F116" t="n">
-        <v>55.55555555555556</v>
+        <v>71.92982456140351</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
         <v>115</v>
       </c>
-      <c r="B117" t="n">
-        <v>6113001685</v>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>6116001059</t>
+        </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL2.decr.19</t>
+          <t>bpop.mn_10..99.MN-DD-UP-OFF2-BL2.incr.39</t>
         </is>
       </c>
       <c r="D117" t="n">
         <v>10</v>
       </c>
       <c r="E117" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F117" t="n">
-        <v>83.33333333333333</v>
+        <v>90.90909090909091</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
         <v>116</v>
       </c>
-      <c r="B118" t="n">
-        <v>6113001685</v>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>6116001059</t>
+        </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL1.decr.20</t>
+          <t>bpop.mn_10..99.MN-DD-UP-OFF2-BL3.incr.38</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E118" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F118" t="n">
-        <v>77.77777777777777</v>
+        <v>66.66666666666667</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
         <v>117</v>
       </c>
-      <c r="B119" t="n">
-        <v>6113001685</v>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>6116001059</t>
+        </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF5-BL2.incr.11</t>
+          <t>bpop.mn_10..99.MN-DD-UP-OFF2-BL4.incr.37</t>
         </is>
       </c>
       <c r="D119" t="n">
         <v>2</v>
       </c>
       <c r="E119" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F119" t="n">
-        <v>66.66666666666667</v>
+        <v>33.33333333333334</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
         <v>118</v>
       </c>
-      <c r="B120" t="n">
-        <v>6113001685</v>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>6116001059</t>
+        </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF5-BL4.decr.25</t>
+          <t>bpop.mn_40..99.MN-DD-UP-OFF1-BL4.decr.49</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E120" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="F120" t="n">
-        <v>95.23809523809524</v>
+        <v>100</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
         <v>119</v>
       </c>
-      <c r="B121" t="n">
-        <v>6113001685</v>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF5-BL3.decr.26</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL2.incr.3</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>12</v>
+        <v>84</v>
       </c>
       <c r="E121" t="n">
-        <v>15</v>
+        <v>134</v>
       </c>
       <c r="F121" t="n">
-        <v>80</v>
+        <v>62.6865671641791</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="B122" t="n">
-        <v>6116001059</v>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>bpop.mn_10..99.MN-DD-UP-OFF2-BL1.incr.40</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL1.incr.4</t>
         </is>
       </c>
       <c r="D122" t="n">
-        <v>41</v>
+        <v>219</v>
       </c>
       <c r="E122" t="n">
-        <v>57</v>
+        <v>379</v>
       </c>
       <c r="F122" t="n">
-        <v>71.92982456140351</v>
+        <v>57.78364116094987</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
         <v>121</v>
       </c>
-      <c r="B123" t="n">
-        <v>6116001059</v>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>bpop.mn_10..99.MN-DD-UP-OFF2-BL2.incr.39</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL3.incr.2</t>
         </is>
       </c>
       <c r="D123" t="n">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="E123" t="n">
-        <v>11</v>
+        <v>174</v>
       </c>
       <c r="F123" t="n">
-        <v>90.90909090909091</v>
+        <v>68.96551724137932</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
         <v>122</v>
       </c>
-      <c r="B124" t="n">
-        <v>6116001059</v>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>bpop.mn_10..99.MN-DD-UP-OFF2-BL3.incr.38</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF2-BL3.incr.6</t>
         </is>
       </c>
       <c r="D124" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E124" t="n">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="F124" t="n">
-        <v>66.66666666666667</v>
+        <v>64.51612903225806</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="B125" t="n">
-        <v>6116001059</v>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>bpop.mn_10..99.MN-DD-UP-OFF2-BL4.incr.37</t>
+          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL4.decr.17</t>
         </is>
       </c>
       <c r="D125" t="n">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="E125" t="n">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="F125" t="n">
-        <v>33.33333333333334</v>
+        <v>63.1578947368421</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
         <v>124</v>
       </c>
-      <c r="B126" t="n">
-        <v>6116001059</v>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>bpop.mn_40..99.MN-DD-UP-OFF1-BL4.decr.49</t>
+          <t>bpop.gl_dot.0..9.GL_SD_OFF1_L.bub2.6</t>
         </is>
       </c>
       <c r="D126" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E126" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="F126" t="n">
-        <v>100</v>
+        <v>71.42857142857143</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
         <v>125</v>
       </c>
-      <c r="B127" t="n">
-        <v>6118002520</v>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL2.incr.3</t>
+          <t>bpop.gl_dot.0..9.GL_SD_OFFW1_L.bub2.8</t>
         </is>
       </c>
       <c r="D127" t="n">
-        <v>84</v>
+        <v>10</v>
       </c>
       <c r="E127" t="n">
-        <v>134</v>
+        <v>14</v>
       </c>
       <c r="F127" t="n">
-        <v>62.6865671641791</v>
+        <v>71.42857142857143</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
         <v>126</v>
       </c>
-      <c r="B128" t="n">
-        <v>6118002520</v>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL1.incr.4</t>
+          <t>bpop.gl_num.0..9.GL_SD_OFF1_M.bub3.13</t>
         </is>
       </c>
       <c r="D128" t="n">
-        <v>219</v>
+        <v>20</v>
       </c>
       <c r="E128" t="n">
-        <v>379</v>
+        <v>43</v>
       </c>
       <c r="F128" t="n">
-        <v>57.78364116094987</v>
+        <v>46.51162790697674</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
         <v>127</v>
       </c>
-      <c r="B129" t="n">
-        <v>6118002520</v>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL3.incr.2</t>
+          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL1.decr.20</t>
         </is>
       </c>
       <c r="D129" t="n">
-        <v>120</v>
+        <v>32</v>
       </c>
       <c r="E129" t="n">
-        <v>174</v>
+        <v>53</v>
       </c>
       <c r="F129" t="n">
-        <v>68.96551724137932</v>
+        <v>60.37735849056604</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
         <v>128</v>
       </c>
-      <c r="B130" t="n">
-        <v>6118002520</v>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF2-BL3.incr.6</t>
+          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL2.decr.19</t>
         </is>
       </c>
       <c r="D130" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E130" t="n">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F130" t="n">
-        <v>64.51612903225806</v>
+        <v>66.66666666666667</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
         <v>129</v>
       </c>
-      <c r="B131" t="n">
-        <v>6118002520</v>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL4.decr.17</t>
+          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL3.decr.18</t>
         </is>
       </c>
       <c r="D131" t="n">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="E131" t="n">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="F131" t="n">
-        <v>63.1578947368421</v>
+        <v>68</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
         <v>130</v>
       </c>
-      <c r="B132" t="n">
-        <v>6118002520</v>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>bpop.gl_dot.0..9.GL_SD_OFF1_L.bub2.6</t>
+          <t>bpop.gl_num.0..9.GL_SD_OFFW1_M.bub3.15</t>
         </is>
       </c>
       <c r="D132" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="E132" t="n">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="F132" t="n">
-        <v>71.42857142857143</v>
+        <v>65.57377049180327</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
         <v>131</v>
       </c>
-      <c r="B133" t="n">
-        <v>6118002520</v>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>bpop.gl_dot.0..9.GL_SD_OFFW1_L.bub2.8</t>
+          <t>bpop.gl_num.0..9.GL_SD_OFFW1_L.bub3.16</t>
         </is>
       </c>
       <c r="D133" t="n">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E133" t="n">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="F133" t="n">
-        <v>71.42857142857143</v>
+        <v>64.86486486486487</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
         <v>132</v>
       </c>
-      <c r="B134" t="n">
-        <v>6118002520</v>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>bpop.gl_num.0..9.GL_SD_OFF1_M.bub3.13</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL4.incr.1</t>
         </is>
       </c>
       <c r="D134" t="n">
-        <v>20</v>
+        <v>58</v>
       </c>
       <c r="E134" t="n">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="F134" t="n">
-        <v>46.51162790697674</v>
+        <v>65.90909090909091</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
         <v>133</v>
       </c>
-      <c r="B135" t="n">
-        <v>6118002520</v>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL1.decr.20</t>
+          <t>bpop.num_0..9.by.1.asc.q2q.AV.rise.12__it_2</t>
         </is>
       </c>
       <c r="D135" t="n">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E135" t="n">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="F135" t="n">
-        <v>60.37735849056604</v>
+        <v>90.90909090909091</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
         <v>134</v>
       </c>
-      <c r="B136" t="n">
-        <v>6118002520</v>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL2.decr.19</t>
+          <t>bpop.num_1..4.by.1.asc.q2q.AV.mc.1</t>
         </is>
       </c>
       <c r="D136" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E136" t="n">
         <v>15</v>
       </c>
       <c r="F136" t="n">
-        <v>66.66666666666667</v>
+        <v>80</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
         <v>135</v>
       </c>
-      <c r="B137" t="n">
-        <v>6118002520</v>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL3.decr.18</t>
+          <t>bpop.num_1..4.by.1.asc.q2q.AV.rise.2</t>
         </is>
       </c>
       <c r="D137" t="n">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="E137" t="n">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="F137" t="n">
-        <v>68</v>
+        <v>90.90909090909091</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
         <v>136</v>
       </c>
-      <c r="B138" t="n">
-        <v>6118002520</v>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>bpop.gl_num.0..9.GL_SD_OFFW1_M.bub3.15</t>
+          <t>bpop.num_0..9.by.1.asc.q2q.AV.mc.11</t>
         </is>
       </c>
       <c r="D138" t="n">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="E138" t="n">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="F138" t="n">
-        <v>65.57377049180327</v>
+        <v>100</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
         <v>137</v>
       </c>
-      <c r="B139" t="n">
-        <v>6118002520</v>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>bpop.gl_num.0..9.GL_SD_OFFW1_L.bub3.16</t>
+          <t>bpop.num_0..9.by.1.asc.q2q.AV.rise.12__it_1</t>
         </is>
       </c>
       <c r="D139" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E139" t="n">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="F139" t="n">
-        <v>64.86486486486487</v>
+        <v>90.90909090909091</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
         <v>138</v>
       </c>
-      <c r="B140" t="n">
-        <v>6118002520</v>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL4.incr.1</t>
+          <t>bpop.num_0..9.by.1.dn.q2q.AV.rise.22</t>
         </is>
       </c>
       <c r="D140" t="n">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="E140" t="n">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="F140" t="n">
-        <v>65.90909090909091</v>
+        <v>90.90909090909091</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
         <v>139</v>
       </c>
-      <c r="B141" t="n">
-        <v>6118002520</v>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.asc.q2q.AV.rise.12__it_2</t>
+          <t>bpop.num_0..9.by.1.rand.q2q.AV.mc.31</t>
         </is>
       </c>
       <c r="D141" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E141" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="F141" t="n">
-        <v>90.90909090909091</v>
+        <v>85.71428571428571</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="B142" t="n">
-        <v>6118002520</v>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>bpop.num_1..4.by.1.asc.q2q.AV.mc.1</t>
+          <t>bpop.num_0..9.by.1.rand.q2q.AV.rise.32</t>
         </is>
       </c>
       <c r="D142" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E142" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F142" t="n">
-        <v>80</v>
+        <v>68.75</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
         <v>141</v>
       </c>
-      <c r="B143" t="n">
-        <v>6118002520</v>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>bpop.num_1..4.by.1.asc.q2q.AV.rise.2</t>
+          <t>bpop.num_1..4.by.1.asc.s2s.AV.mc.7</t>
         </is>
       </c>
       <c r="D143" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E143" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F143" t="n">
-        <v>90.90909090909091</v>
+        <v>78.94736842105263</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
         <v>142</v>
       </c>
-      <c r="B144" t="n">
-        <v>6118002520</v>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.asc.q2q.AV.mc.11</t>
+          <t>bpop.num_1..4.by.1.asc.s2s.AV.rise.8</t>
         </is>
       </c>
       <c r="D144" t="n">
         <v>10</v>
       </c>
       <c r="E144" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F144" t="n">
-        <v>100</v>
+        <v>90.90909090909091</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
         <v>143</v>
       </c>
-      <c r="B145" t="n">
-        <v>6118002520</v>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.asc.q2q.AV.rise.12__it_1</t>
+          <t>bpop.num_1..4.by.1.asc.x2s.Ax.mc.9</t>
         </is>
       </c>
       <c r="D145" t="n">
         <v>10</v>
       </c>
       <c r="E145" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F145" t="n">
-        <v>90.90909090909091</v>
+        <v>100</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
         <v>144</v>
       </c>
-      <c r="B146" t="n">
-        <v>6118002520</v>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.dn.q2q.AV.rise.22</t>
+          <t>bpop.num_0..9.by.1.asc.s2s.AV.mc.17</t>
         </is>
       </c>
       <c r="D146" t="n">
@@ -3743,100 +3877,110 @@
       <c r="A147" s="1" t="n">
         <v>145</v>
       </c>
-      <c r="B147" t="n">
-        <v>6118002520</v>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.rand.q2q.AV.mc.31</t>
+          <t>bpop.num_0..9.by.1.asc.x2s.Ax.mc.19</t>
         </is>
       </c>
       <c r="D147" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E147" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F147" t="n">
-        <v>85.71428571428571</v>
+        <v>90.90909090909091</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
         <v>146</v>
       </c>
-      <c r="B148" t="n">
-        <v>6118002520</v>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.rand.q2q.AV.rise.32</t>
+          <t>bpop.num_0..9.by.1.dn.s2s.AV.mc.27</t>
         </is>
       </c>
       <c r="D148" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E148" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="F148" t="n">
-        <v>68.75</v>
+        <v>100</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
         <v>147</v>
       </c>
-      <c r="B149" t="n">
-        <v>6118002520</v>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>bpop.num_1..4.by.1.asc.s2s.AV.mc.7</t>
+          <t>bpop.num_0..9.by.1.dn.x2s.Ax.mc.29</t>
         </is>
       </c>
       <c r="D149" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E149" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F149" t="n">
-        <v>78.94736842105263</v>
+        <v>83.33333333333333</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
         <v>148</v>
       </c>
-      <c r="B150" t="n">
-        <v>6118002520</v>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>bpop.num_1..4.by.1.asc.s2s.AV.rise.8</t>
+          <t>bpop.num_0..9.by.1.dn.x2s.Ax.rise.30</t>
         </is>
       </c>
       <c r="D150" t="n">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="E150" t="n">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="F150" t="n">
-        <v>90.90909090909091</v>
+        <v>72.72727272727273</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
         <v>149</v>
       </c>
-      <c r="B151" t="n">
-        <v>6118002520</v>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>bpop.num_1..4.by.1.asc.x2s.Ax.mc.9</t>
+          <t>bpop.num_0..9.by.1.rand.s2s.AV.mc.37</t>
         </is>
       </c>
       <c r="D151" t="n">
@@ -3853,122 +3997,134 @@
       <c r="A152" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="B152" t="n">
-        <v>6118002520</v>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.asc.s2s.AV.mc.17</t>
+          <t>bpop.num_0..9.by.1.rand.s2s.AV.rise.38</t>
         </is>
       </c>
       <c r="D152" t="n">
         <v>10</v>
       </c>
       <c r="E152" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F152" t="n">
-        <v>90.90909090909091</v>
+        <v>83.33333333333333</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="B153" t="n">
-        <v>6118002520</v>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.asc.x2s.Ax.mc.19</t>
+          <t>bpop.num_0..9.by.1.rand.x2s.Ax.mc.39</t>
         </is>
       </c>
       <c r="D153" t="n">
         <v>10</v>
       </c>
       <c r="E153" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F153" t="n">
-        <v>90.90909090909091</v>
+        <v>100</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
         <v>152</v>
       </c>
-      <c r="B154" t="n">
-        <v>6118002520</v>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.dn.s2s.AV.mc.27</t>
+          <t>bpop.num_0..9.by.1.rand.x2s.Ax.rise.42__it_1</t>
         </is>
       </c>
       <c r="D154" t="n">
         <v>10</v>
       </c>
       <c r="E154" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F154" t="n">
-        <v>100</v>
+        <v>76.92307692307692</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
         <v>153</v>
       </c>
-      <c r="B155" t="n">
-        <v>6118002520</v>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.dn.x2s.Ax.mc.29</t>
+          <t>bpop.num_1..4.by.1.asc.q2s.AV.rise.4</t>
         </is>
       </c>
       <c r="D155" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E155" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F155" t="n">
-        <v>83.33333333333333</v>
+        <v>68.18181818181819</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
         <v>154</v>
       </c>
-      <c r="B156" t="n">
-        <v>6118002520</v>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.dn.x2s.Ax.rise.30</t>
+          <t>bpop.num_0..9.by.1.asc.q2s.AV.mc.13</t>
         </is>
       </c>
       <c r="D156" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="E156" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="F156" t="n">
-        <v>72.72727272727273</v>
+        <v>100</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
         <v>155</v>
       </c>
-      <c r="B157" t="n">
-        <v>6118002520</v>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.rand.s2s.AV.mc.37</t>
+          <t>bpop.num_0..9.by.1.dn.q2s.AV.rise.24</t>
         </is>
       </c>
       <c r="D157" t="n">
@@ -3985,122 +4141,134 @@
       <c r="A158" s="1" t="n">
         <v>156</v>
       </c>
-      <c r="B158" t="n">
-        <v>6118002520</v>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.rand.s2s.AV.rise.38</t>
+          <t>bpop.num_0..9.by.1.rand.q2s.AV.mc.33</t>
         </is>
       </c>
       <c r="D158" t="n">
         <v>10</v>
       </c>
       <c r="E158" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F158" t="n">
-        <v>83.33333333333333</v>
+        <v>100</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
         <v>157</v>
       </c>
-      <c r="B159" t="n">
-        <v>6118002520</v>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.rand.x2s.Ax.mc.39</t>
+          <t>bpop.num_1..4.by.1.asc.s2q.AV.mc.5</t>
         </is>
       </c>
       <c r="D159" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E159" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F159" t="n">
-        <v>100</v>
+        <v>95.23809523809524</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
         <v>158</v>
       </c>
-      <c r="B160" t="n">
-        <v>6118002520</v>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.rand.x2s.Ax.rise.42__it_1</t>
+          <t>bpop.num_0..9.by.1.asc.s2q.AV.rise.16</t>
         </is>
       </c>
       <c r="D160" t="n">
         <v>10</v>
       </c>
       <c r="E160" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F160" t="n">
-        <v>76.92307692307692</v>
+        <v>83.33333333333333</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
         <v>159</v>
       </c>
-      <c r="B161" t="n">
-        <v>6118002520</v>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>bpop.num_1..4.by.1.asc.q2s.AV.rise.4</t>
+          <t>bpop.num_0..9.by.1.dn.s2q.AV.mc.25</t>
         </is>
       </c>
       <c r="D161" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E161" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="F161" t="n">
-        <v>68.18181818181819</v>
+        <v>83.33333333333333</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
         <v>160</v>
       </c>
-      <c r="B162" t="n">
-        <v>6118002520</v>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.asc.q2s.AV.mc.13</t>
+          <t>bpop.num_0..9.by.1.dn.s2q.AV.rise.26</t>
         </is>
       </c>
       <c r="D162" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E162" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="F162" t="n">
-        <v>100</v>
+        <v>63.33333333333334</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
         <v>161</v>
       </c>
-      <c r="B163" t="n">
-        <v>6118002520</v>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.dn.q2s.AV.rise.24</t>
+          <t>bpop.num_0..9.by.1.rand.s2q.AV.mc.35</t>
         </is>
       </c>
       <c r="D163" t="n">
@@ -4117,12 +4285,14 @@
       <c r="A164" s="1" t="n">
         <v>162</v>
       </c>
-      <c r="B164" t="n">
-        <v>6118002520</v>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>6118002520</t>
+        </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.rand.q2s.AV.mc.33</t>
+          <t>bpop.num_0..9.by.1.rand.x2s.Ax.rise.42__it_2</t>
         </is>
       </c>
       <c r="D164" t="n">
@@ -4139,307 +4309,191 @@
       <c r="A165" s="1" t="n">
         <v>163</v>
       </c>
-      <c r="B165" t="n">
-        <v>6118002520</v>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>6118003400</t>
+        </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>bpop.num_1..4.by.1.asc.s2q.AV.mc.5</t>
+          <t>bpop.num_0..9.by.1.asc.q2q.AV.rise.12__it_2</t>
         </is>
       </c>
       <c r="D165" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E165" t="n">
         <v>21</v>
       </c>
       <c r="F165" t="n">
-        <v>95.23809523809524</v>
+        <v>23.80952380952381</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
         <v>164</v>
       </c>
-      <c r="B166" t="n">
-        <v>6118002520</v>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>6118003535</t>
+        </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.asc.s2q.AV.rise.16</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL4.incr.1</t>
         </is>
       </c>
       <c r="D166" t="n">
         <v>10</v>
       </c>
       <c r="E166" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F166" t="n">
-        <v>83.33333333333333</v>
+        <v>100</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
         <v>165</v>
       </c>
-      <c r="B167" t="n">
-        <v>6118002520</v>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>6118003535</t>
+        </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.dn.s2q.AV.mc.25</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL2.incr.3</t>
         </is>
       </c>
       <c r="D167" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E167" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F167" t="n">
-        <v>83.33333333333333</v>
+        <v>100</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
         <v>166</v>
       </c>
-      <c r="B168" t="n">
-        <v>6118002520</v>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>6118003535</t>
+        </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.dn.s2q.AV.rise.26</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL3.incr.2</t>
         </is>
       </c>
       <c r="D168" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E168" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="F168" t="n">
-        <v>63.33333333333334</v>
+        <v>90.90909090909091</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
         <v>167</v>
       </c>
-      <c r="B169" t="n">
-        <v>6118002520</v>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>6118003535</t>
+        </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.rand.s2q.AV.mc.35</t>
+          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL1.incr.4</t>
         </is>
       </c>
       <c r="D169" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E169" t="n">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="F169" t="n">
-        <v>100</v>
+        <v>64.51612903225806</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
         <v>168</v>
       </c>
-      <c r="B170" t="n">
-        <v>6118002520</v>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>6118003535</t>
+        </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.rand.x2s.Ax.rise.42__it_2</t>
+          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL4.decr.17</t>
         </is>
       </c>
       <c r="D170" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E170" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F170" t="n">
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
         <v>169</v>
       </c>
-      <c r="B171" t="n">
-        <v>6118003400</v>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>6118003535</t>
+        </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>bpop.num_0..9.by.1.asc.q2q.AV.rise.12__it_2</t>
+          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL3.decr.18</t>
         </is>
       </c>
       <c r="D171" t="n">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="E171" t="n">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="F171" t="n">
-        <v>23.80952380952381</v>
+        <v>70</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
         <v>170</v>
       </c>
-      <c r="B172" t="n">
-        <v>6118003535</v>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>6118003535</t>
+        </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL4.incr.1</t>
+          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL2.decr.19</t>
         </is>
       </c>
       <c r="D172" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E172" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F172" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" s="1" t="n">
-        <v>171</v>
-      </c>
-      <c r="B173" t="n">
-        <v>6118003535</v>
-      </c>
-      <c r="C173" t="inlineStr">
-        <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL2.incr.3</t>
-        </is>
-      </c>
-      <c r="D173" t="n">
-        <v>1</v>
-      </c>
-      <c r="E173" t="n">
-        <v>1</v>
-      </c>
-      <c r="F173" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" s="1" t="n">
-        <v>172</v>
-      </c>
-      <c r="B174" t="n">
-        <v>6118003535</v>
-      </c>
-      <c r="C174" t="inlineStr">
-        <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL3.incr.2</t>
-        </is>
-      </c>
-      <c r="D174" t="n">
-        <v>10</v>
-      </c>
-      <c r="E174" t="n">
-        <v>11</v>
-      </c>
-      <c r="F174" t="n">
-        <v>90.90909090909091</v>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" s="1" t="n">
-        <v>173</v>
-      </c>
-      <c r="B175" t="n">
-        <v>6118003535</v>
-      </c>
-      <c r="C175" t="inlineStr">
-        <is>
-          <t>bpop.mn_0..9.MN-SD-UP-OFF1-BL1.incr.4</t>
-        </is>
-      </c>
-      <c r="D175" t="n">
-        <v>20</v>
-      </c>
-      <c r="E175" t="n">
-        <v>31</v>
-      </c>
-      <c r="F175" t="n">
-        <v>64.51612903225806</v>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" s="1" t="n">
-        <v>174</v>
-      </c>
-      <c r="B176" t="n">
-        <v>6118003535</v>
-      </c>
-      <c r="C176" t="inlineStr">
-        <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL4.decr.17</t>
-        </is>
-      </c>
-      <c r="D176" t="n">
-        <v>9</v>
-      </c>
-      <c r="E176" t="n">
-        <v>15</v>
-      </c>
-      <c r="F176" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" s="1" t="n">
-        <v>175</v>
-      </c>
-      <c r="B177" t="n">
-        <v>6118003535</v>
-      </c>
-      <c r="C177" t="inlineStr">
-        <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL3.decr.18</t>
-        </is>
-      </c>
-      <c r="D177" t="n">
-        <v>35</v>
-      </c>
-      <c r="E177" t="n">
-        <v>50</v>
-      </c>
-      <c r="F177" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" s="1" t="n">
-        <v>176</v>
-      </c>
-      <c r="B178" t="n">
-        <v>6118003535</v>
-      </c>
-      <c r="C178" t="inlineStr">
-        <is>
-          <t>bpop.mn_4..9.MN-SD-UP-OFF1-BL2.decr.19</t>
-        </is>
-      </c>
-      <c r="D178" t="n">
-        <v>11</v>
-      </c>
-      <c r="E178" t="n">
-        <v>17</v>
-      </c>
-      <c r="F178" t="n">
         <v>64.70588235294117</v>
       </c>
     </row>

</xml_diff>